<commit_message>
Chamada do dia 24/08/2025
</commit_message>
<xml_diff>
--- a/chamada.xlsx
+++ b/chamada.xlsx
@@ -415,7 +415,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H226"/>
+  <dimension ref="A1:H256"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A193" workbookViewId="0">
       <selection activeCell="B214" sqref="B214"/>
@@ -4270,6 +4270,516 @@
       <c r="C226" t="inlineStr">
         <is>
           <t>10/08/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="227">
+      <c r="A227" t="inlineStr">
+        <is>
+          <t>OsValdina Francisca</t>
+        </is>
+      </c>
+      <c r="B227" t="inlineStr">
+        <is>
+          <t>Presente</t>
+        </is>
+      </c>
+      <c r="C227" t="inlineStr">
+        <is>
+          <t>17/08/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="228">
+      <c r="A228" t="inlineStr">
+        <is>
+          <t>Paulo Henrique</t>
+        </is>
+      </c>
+      <c r="B228" t="inlineStr">
+        <is>
+          <t>Ausente</t>
+        </is>
+      </c>
+      <c r="C228" t="inlineStr">
+        <is>
+          <t>17/08/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="229">
+      <c r="A229" t="inlineStr">
+        <is>
+          <t>João Vitor</t>
+        </is>
+      </c>
+      <c r="B229" t="inlineStr">
+        <is>
+          <t>Presente</t>
+        </is>
+      </c>
+      <c r="C229" t="inlineStr">
+        <is>
+          <t>17/08/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="230">
+      <c r="A230" t="inlineStr">
+        <is>
+          <t>Elza Alves</t>
+        </is>
+      </c>
+      <c r="B230" t="inlineStr">
+        <is>
+          <t>Presente</t>
+        </is>
+      </c>
+      <c r="C230" t="inlineStr">
+        <is>
+          <t>17/08/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="231">
+      <c r="A231" t="inlineStr">
+        <is>
+          <t>Antonio Patricio</t>
+        </is>
+      </c>
+      <c r="B231" t="inlineStr">
+        <is>
+          <t>Presente</t>
+        </is>
+      </c>
+      <c r="C231" t="inlineStr">
+        <is>
+          <t>17/08/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="232">
+      <c r="A232" t="inlineStr">
+        <is>
+          <t>Gesmindo Boostel</t>
+        </is>
+      </c>
+      <c r="B232" t="inlineStr">
+        <is>
+          <t>Presente</t>
+        </is>
+      </c>
+      <c r="C232" t="inlineStr">
+        <is>
+          <t>17/08/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="233">
+      <c r="A233" t="inlineStr">
+        <is>
+          <t>Kalahan Boostel</t>
+        </is>
+      </c>
+      <c r="B233" t="inlineStr">
+        <is>
+          <t>Presente</t>
+        </is>
+      </c>
+      <c r="C233" t="inlineStr">
+        <is>
+          <t>17/08/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="234">
+      <c r="A234" t="inlineStr">
+        <is>
+          <t>Geciel Polegario</t>
+        </is>
+      </c>
+      <c r="B234" t="inlineStr">
+        <is>
+          <t>Presente</t>
+        </is>
+      </c>
+      <c r="C234" t="inlineStr">
+        <is>
+          <t>17/08/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="235">
+      <c r="A235" t="inlineStr">
+        <is>
+          <t>Diana</t>
+        </is>
+      </c>
+      <c r="B235" t="inlineStr">
+        <is>
+          <t>Ausente</t>
+        </is>
+      </c>
+      <c r="C235" t="inlineStr">
+        <is>
+          <t>17/08/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="236">
+      <c r="A236" t="inlineStr">
+        <is>
+          <t>Vanuza Nascimento</t>
+        </is>
+      </c>
+      <c r="B236" t="inlineStr">
+        <is>
+          <t>Presente</t>
+        </is>
+      </c>
+      <c r="C236" t="inlineStr">
+        <is>
+          <t>17/08/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="237">
+      <c r="A237" t="inlineStr">
+        <is>
+          <t>Welington Nascimento</t>
+        </is>
+      </c>
+      <c r="B237" t="inlineStr">
+        <is>
+          <t>Ausente</t>
+        </is>
+      </c>
+      <c r="C237" t="inlineStr">
+        <is>
+          <t>17/08/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="238">
+      <c r="A238" t="inlineStr">
+        <is>
+          <t>Welington Ribeiro</t>
+        </is>
+      </c>
+      <c r="B238" t="inlineStr">
+        <is>
+          <t>Ausente</t>
+        </is>
+      </c>
+      <c r="C238" t="inlineStr">
+        <is>
+          <t>17/08/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="239">
+      <c r="A239" t="inlineStr">
+        <is>
+          <t>Jorge</t>
+        </is>
+      </c>
+      <c r="B239" t="inlineStr">
+        <is>
+          <t>Presente</t>
+        </is>
+      </c>
+      <c r="C239" t="inlineStr">
+        <is>
+          <t>17/08/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="240">
+      <c r="A240" t="inlineStr">
+        <is>
+          <t>Gosmira</t>
+        </is>
+      </c>
+      <c r="B240" t="inlineStr">
+        <is>
+          <t>Presente</t>
+        </is>
+      </c>
+      <c r="C240" t="inlineStr">
+        <is>
+          <t>17/08/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="241">
+      <c r="A241" t="inlineStr">
+        <is>
+          <t>Almir Rodrigues</t>
+        </is>
+      </c>
+      <c r="B241" t="inlineStr">
+        <is>
+          <t>Presente</t>
+        </is>
+      </c>
+      <c r="C241" t="inlineStr">
+        <is>
+          <t>17/08/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="242">
+      <c r="A242" t="inlineStr">
+        <is>
+          <t>OsValdina Francisca</t>
+        </is>
+      </c>
+      <c r="B242" t="inlineStr">
+        <is>
+          <t>Presente</t>
+        </is>
+      </c>
+      <c r="C242" t="inlineStr">
+        <is>
+          <t>24/08/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="243">
+      <c r="A243" t="inlineStr">
+        <is>
+          <t>Paulo Henrique</t>
+        </is>
+      </c>
+      <c r="B243" t="inlineStr">
+        <is>
+          <t>Ausente</t>
+        </is>
+      </c>
+      <c r="C243" t="inlineStr">
+        <is>
+          <t>24/08/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="244">
+      <c r="A244" t="inlineStr">
+        <is>
+          <t>João Vitor</t>
+        </is>
+      </c>
+      <c r="B244" t="inlineStr">
+        <is>
+          <t>Ausente</t>
+        </is>
+      </c>
+      <c r="C244" t="inlineStr">
+        <is>
+          <t>24/08/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="245">
+      <c r="A245" t="inlineStr">
+        <is>
+          <t>Elza Alves</t>
+        </is>
+      </c>
+      <c r="B245" t="inlineStr">
+        <is>
+          <t>Presente</t>
+        </is>
+      </c>
+      <c r="C245" t="inlineStr">
+        <is>
+          <t>24/08/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="246">
+      <c r="A246" t="inlineStr">
+        <is>
+          <t>Antonio Patricio</t>
+        </is>
+      </c>
+      <c r="B246" t="inlineStr">
+        <is>
+          <t>Presente</t>
+        </is>
+      </c>
+      <c r="C246" t="inlineStr">
+        <is>
+          <t>24/08/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="247">
+      <c r="A247" t="inlineStr">
+        <is>
+          <t>Gesmindo Boostel</t>
+        </is>
+      </c>
+      <c r="B247" t="inlineStr">
+        <is>
+          <t>Presente</t>
+        </is>
+      </c>
+      <c r="C247" t="inlineStr">
+        <is>
+          <t>24/08/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="248">
+      <c r="A248" t="inlineStr">
+        <is>
+          <t>Kalahan Boostel</t>
+        </is>
+      </c>
+      <c r="B248" t="inlineStr">
+        <is>
+          <t>Presente</t>
+        </is>
+      </c>
+      <c r="C248" t="inlineStr">
+        <is>
+          <t>24/08/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="249">
+      <c r="A249" t="inlineStr">
+        <is>
+          <t>Geciel Polegario</t>
+        </is>
+      </c>
+      <c r="B249" t="inlineStr">
+        <is>
+          <t>Ausente</t>
+        </is>
+      </c>
+      <c r="C249" t="inlineStr">
+        <is>
+          <t>24/08/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="250">
+      <c r="A250" t="inlineStr">
+        <is>
+          <t>Diana</t>
+        </is>
+      </c>
+      <c r="B250" t="inlineStr">
+        <is>
+          <t>Ausente</t>
+        </is>
+      </c>
+      <c r="C250" t="inlineStr">
+        <is>
+          <t>24/08/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="251">
+      <c r="A251" t="inlineStr">
+        <is>
+          <t>Vanuza Nascimento</t>
+        </is>
+      </c>
+      <c r="B251" t="inlineStr">
+        <is>
+          <t>Ausente</t>
+        </is>
+      </c>
+      <c r="C251" t="inlineStr">
+        <is>
+          <t>24/08/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="252">
+      <c r="A252" t="inlineStr">
+        <is>
+          <t>Welington Nascimento</t>
+        </is>
+      </c>
+      <c r="B252" t="inlineStr">
+        <is>
+          <t>Ausente</t>
+        </is>
+      </c>
+      <c r="C252" t="inlineStr">
+        <is>
+          <t>24/08/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="253">
+      <c r="A253" t="inlineStr">
+        <is>
+          <t>Welington Ribeiro</t>
+        </is>
+      </c>
+      <c r="B253" t="inlineStr">
+        <is>
+          <t>Ausente</t>
+        </is>
+      </c>
+      <c r="C253" t="inlineStr">
+        <is>
+          <t>24/08/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="254">
+      <c r="A254" t="inlineStr">
+        <is>
+          <t>Jorge</t>
+        </is>
+      </c>
+      <c r="B254" t="inlineStr">
+        <is>
+          <t>Ausente</t>
+        </is>
+      </c>
+      <c r="C254" t="inlineStr">
+        <is>
+          <t>24/08/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="255">
+      <c r="A255" t="inlineStr">
+        <is>
+          <t>Gosmira</t>
+        </is>
+      </c>
+      <c r="B255" t="inlineStr">
+        <is>
+          <t>Ausente</t>
+        </is>
+      </c>
+      <c r="C255" t="inlineStr">
+        <is>
+          <t>24/08/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="256">
+      <c r="A256" t="inlineStr">
+        <is>
+          <t>Almir Rodrigues</t>
+        </is>
+      </c>
+      <c r="B256" t="inlineStr">
+        <is>
+          <t>Presente</t>
+        </is>
+      </c>
+      <c r="C256" t="inlineStr">
+        <is>
+          <t>24/08/2025</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Modificação do codigo que recebeu atualização para exclusão de nome, assim que o nome correto ´digitado, ele some da lista automaticamente
</commit_message>
<xml_diff>
--- a/chamada.xlsx
+++ b/chamada.xlsx
@@ -415,7 +415,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H256"/>
+  <dimension ref="A1:H273"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A193" workbookViewId="0">
       <selection activeCell="B214" sqref="B214"/>
@@ -4780,6 +4780,295 @@
       <c r="C256" t="inlineStr">
         <is>
           <t>24/08/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="257">
+      <c r="A257" t="inlineStr">
+        <is>
+          <t>OsValdina Francisca</t>
+        </is>
+      </c>
+      <c r="B257" t="inlineStr">
+        <is>
+          <t>Presente</t>
+        </is>
+      </c>
+      <c r="C257" t="inlineStr">
+        <is>
+          <t>31/08/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="258">
+      <c r="A258" t="inlineStr">
+        <is>
+          <t>Paulo Henrique</t>
+        </is>
+      </c>
+      <c r="B258" t="inlineStr">
+        <is>
+          <t>Presente</t>
+        </is>
+      </c>
+      <c r="C258" t="inlineStr">
+        <is>
+          <t>31/08/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="259">
+      <c r="A259" t="inlineStr">
+        <is>
+          <t>João Vitor</t>
+        </is>
+      </c>
+      <c r="B259" t="inlineStr">
+        <is>
+          <t>Ausente</t>
+        </is>
+      </c>
+      <c r="C259" t="inlineStr">
+        <is>
+          <t>31/08/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="260">
+      <c r="A260" t="inlineStr">
+        <is>
+          <t>Elza Alves</t>
+        </is>
+      </c>
+      <c r="B260" t="inlineStr">
+        <is>
+          <t>Presente</t>
+        </is>
+      </c>
+      <c r="C260" t="inlineStr">
+        <is>
+          <t>31/08/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="261">
+      <c r="A261" t="inlineStr">
+        <is>
+          <t>Antonio Patricio</t>
+        </is>
+      </c>
+      <c r="B261" t="inlineStr">
+        <is>
+          <t>Presente</t>
+        </is>
+      </c>
+      <c r="C261" t="inlineStr">
+        <is>
+          <t>31/08/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="262">
+      <c r="A262" t="inlineStr">
+        <is>
+          <t>Gesmindo Boostel</t>
+        </is>
+      </c>
+      <c r="B262" t="inlineStr">
+        <is>
+          <t>Presente</t>
+        </is>
+      </c>
+      <c r="C262" t="inlineStr">
+        <is>
+          <t>31/08/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="263">
+      <c r="A263" t="inlineStr">
+        <is>
+          <t>Kalahan Boostel</t>
+        </is>
+      </c>
+      <c r="B263" t="inlineStr">
+        <is>
+          <t>Presente</t>
+        </is>
+      </c>
+      <c r="C263" t="inlineStr">
+        <is>
+          <t>31/08/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="264">
+      <c r="A264" t="inlineStr">
+        <is>
+          <t>Geciel Polegario</t>
+        </is>
+      </c>
+      <c r="B264" t="inlineStr">
+        <is>
+          <t>Presente</t>
+        </is>
+      </c>
+      <c r="C264" t="inlineStr">
+        <is>
+          <t>31/08/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="265">
+      <c r="A265" t="inlineStr">
+        <is>
+          <t>Diana</t>
+        </is>
+      </c>
+      <c r="B265" t="inlineStr">
+        <is>
+          <t>Presente</t>
+        </is>
+      </c>
+      <c r="C265" t="inlineStr">
+        <is>
+          <t>31/08/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="266">
+      <c r="A266" t="inlineStr">
+        <is>
+          <t>Vanuza Nascimento</t>
+        </is>
+      </c>
+      <c r="B266" t="inlineStr">
+        <is>
+          <t>Presente</t>
+        </is>
+      </c>
+      <c r="C266" t="inlineStr">
+        <is>
+          <t>31/08/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="267">
+      <c r="A267" t="inlineStr">
+        <is>
+          <t>Welington Nascimento</t>
+        </is>
+      </c>
+      <c r="B267" t="inlineStr">
+        <is>
+          <t>Presente</t>
+        </is>
+      </c>
+      <c r="C267" t="inlineStr">
+        <is>
+          <t>31/08/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="268">
+      <c r="A268" t="inlineStr">
+        <is>
+          <t>Jorge</t>
+        </is>
+      </c>
+      <c r="B268" t="inlineStr">
+        <is>
+          <t>Ausente</t>
+        </is>
+      </c>
+      <c r="C268" t="inlineStr">
+        <is>
+          <t>31/08/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="269">
+      <c r="A269" t="inlineStr">
+        <is>
+          <t>Gosmira</t>
+        </is>
+      </c>
+      <c r="B269" t="inlineStr">
+        <is>
+          <t>Ausente</t>
+        </is>
+      </c>
+      <c r="C269" t="inlineStr">
+        <is>
+          <t>31/08/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="270">
+      <c r="A270" t="inlineStr">
+        <is>
+          <t>Almir Rodrigues</t>
+        </is>
+      </c>
+      <c r="B270" t="inlineStr">
+        <is>
+          <t>Presente</t>
+        </is>
+      </c>
+      <c r="C270" t="inlineStr">
+        <is>
+          <t>31/08/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="271">
+      <c r="A271" t="inlineStr">
+        <is>
+          <t>Herminio</t>
+        </is>
+      </c>
+      <c r="B271" t="inlineStr">
+        <is>
+          <t>Presente</t>
+        </is>
+      </c>
+      <c r="C271" t="inlineStr">
+        <is>
+          <t>31/08/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="272">
+      <c r="A272" t="inlineStr">
+        <is>
+          <t>Maria do Carmo</t>
+        </is>
+      </c>
+      <c r="B272" t="inlineStr">
+        <is>
+          <t>Presente</t>
+        </is>
+      </c>
+      <c r="C272" t="inlineStr">
+        <is>
+          <t>31/08/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="273">
+      <c r="A273" t="inlineStr">
+        <is>
+          <t>Laide</t>
+        </is>
+      </c>
+      <c r="B273" t="inlineStr">
+        <is>
+          <t>Presente</t>
+        </is>
+      </c>
+      <c r="C273" t="inlineStr">
+        <is>
+          <t>31/08/2025</t>
         </is>
       </c>
     </row>

</xml_diff>